<commit_message>
Corrected the whitebox tests
</commit_message>
<xml_diff>
--- a/FlowChart.xlsx
+++ b/FlowChart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gary\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omega\Desktop\Software\Software CA\Whitebox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0962C7B3-DA2D-497C-9E58-F4BC18C4D2C4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA36FC0A-316F-4573-9459-DB884D119CB3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E8BBE373-386B-417D-A696-0CB2B345258F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8BBE373-386B-417D-A696-0CB2B345258F}"/>
   </bookViews>
   <sheets>
     <sheet name="CA Flowchart" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
     <t>Test_01</t>
   </si>
@@ -92,12 +92,6 @@
     <t>Equivalence Partitioning</t>
   </si>
   <si>
-    <t xml:space="preserve">age    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender           </t>
-  </si>
-  <si>
     <t xml:space="preserve">male             </t>
   </si>
   <si>
@@ -154,6 +148,9 @@
   <si>
     <t>integer</t>
   </si>
+  <si>
+    <t xml:space="preserve">gender </t>
+  </si>
 </sst>
 </file>
 
@@ -177,30 +174,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -214,8 +187,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,8 +223,41 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -237,27 +265,143 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="20% - Accent3" xfId="4" builtinId="38"/>
+    <cellStyle name="20% - Accent4" xfId="5" builtinId="42"/>
+    <cellStyle name="40% - Accent5" xfId="6" builtinId="47"/>
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4667,7 +4811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F1D746-DDB4-4B42-BB3F-398466B07FF1}">
   <dimension ref="B5:B77"/>
   <sheetViews>
-    <sheetView zoomScale="62" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
       <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
@@ -4752,7 +4896,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4761,168 +4905,168 @@
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" customWidth="1"/>
     <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="13">
         <v>18</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="13">
         <v>50</v>
       </c>
-      <c r="D3" s="3">
-        <v>2.875</v>
+      <c r="D3" s="13">
+        <v>1.75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="13">
         <v>31</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="13">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="13">
+        <v>15</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="14"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="12">
+        <v>18</v>
+      </c>
+      <c r="D7" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="12">
+        <v>50</v>
+      </c>
+      <c r="D8" s="12">
         <v>2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="12">
+        <v>36</v>
+      </c>
+      <c r="D9" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="12">
         <v>15</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D10" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3">
-        <v>18</v>
-      </c>
-      <c r="D7" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+      <c r="D11" s="14"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="11">
+        <v>25</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="11">
         <v>50</v>
       </c>
-      <c r="D8" s="3">
-        <v>5.75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="3">
-        <v>36</v>
-      </c>
-      <c r="D9" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3">
-        <v>15</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="3">
-        <v>25</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="3">
-        <v>50</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="D13" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4939,8 +5083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CCDBB22-29C1-4E1E-A596-4094F2DFE512}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4950,365 +5094,406 @@
     <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2">
+        <v>31</v>
+      </c>
+      <c r="D5" s="8">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2">
+        <v>17</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2">
+        <v>50</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="2">
+        <v>19</v>
+      </c>
+      <c r="D9" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="B10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="2">
+        <v>37</v>
+      </c>
+      <c r="D10" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4">
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2">
+        <v>17</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2">
+        <v>50</v>
+      </c>
+      <c r="D12" s="8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>17</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="7">
+      <c r="C22" s="8">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>18</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="8">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>19</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="8">
+        <v>6</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>35</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="8">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>36</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>49</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="8">
+        <v>5</v>
+      </c>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>50</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>17</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="8">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>18</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="8">
+        <v>5</v>
+      </c>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>19</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="8">
+        <v>5</v>
+      </c>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>29</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="8">
+        <v>5</v>
+      </c>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>30</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>31</v>
       </c>
-      <c r="D5" s="7">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6">
-        <v>17</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7">
+      <c r="B35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>49</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
         <v>50</v>
       </c>
-      <c r="D7" s="7">
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9">
-        <v>19</v>
-      </c>
-      <c r="D9" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10">
-        <v>37</v>
-      </c>
-      <c r="D10" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11">
-        <v>17</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12">
-        <v>50</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>17</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="B37" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>18</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C37" s="8">
+        <v>1.75</v>
+      </c>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>51</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>19</v>
-      </c>
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>35</v>
-      </c>
-      <c r="B25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>36</v>
-      </c>
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>49</v>
-      </c>
-      <c r="B27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>50</v>
-      </c>
-      <c r="B28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="7">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>17</v>
-      </c>
-      <c r="B30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>18</v>
-      </c>
-      <c r="B31" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>19</v>
-      </c>
-      <c r="B32" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>29</v>
-      </c>
-      <c r="B33" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>30</v>
-      </c>
-      <c r="B34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="7">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>31</v>
-      </c>
-      <c r="B35" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="7">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>49</v>
-      </c>
-      <c r="B36" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="7">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>50</v>
-      </c>
-      <c r="B37" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" s="7">
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>51</v>
-      </c>
-      <c r="B38" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="7">
-        <v>0.375</v>
-      </c>
+      <c r="C38" s="8">
+        <v>1.75</v>
+      </c>
+      <c r="D38" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>